<commit_message>
Update NaCl NIOSH Test Results 13 Apr 2020 WNg et al.xlsx
</commit_message>
<xml_diff>
--- a/04-Testing/NaCl NIOSH Test Results 13 Apr 2020 WNg et al.xlsx
+++ b/04-Testing/NaCl NIOSH Test Results 13 Apr 2020 WNg et al.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wckng/Documents/GitHub/Reusable-N95-Project/04-Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45958C13-265F-E54C-BB1E-5CB7ABC086E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFB4486-0628-8D43-97EF-28D103459859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{2B97CAC9-7827-284E-8A55-0F6A34A68828}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>NaCl NIOSH Testing 13 April 11am to 3pm at James Scott Lab</t>
   </si>
@@ -52,6 +53,9 @@
   </si>
   <si>
     <t>Attendees: Andrew Syrett, Vahid Anwari, Will Ng, Matt Ratto</t>
+  </si>
+  <si>
+    <t>Problems</t>
   </si>
 </sst>
 </file>
@@ -412,25 +416,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D5A731-0550-CF4C-A035-1CCCFCB236F8}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -443,28 +447,29 @@
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>

</xml_diff>